<commit_message>
Fix index refresh bugs
</commit_message>
<xml_diff>
--- a/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes-v2.xlsx
+++ b/federation/src/main/webapp/theme-default/shapes/OpenArchaeo-Shapes-v2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\MASA\01-OpenArchaeo\20-Sources\openarchaeo\federation\src\main\webapp\theme-default\shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA630E-D451-4C93-A033-8E9A8F44A832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1162E-ADF2-4170-B386-D9F2AD7948C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14355" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <t>crm:E53_Place</t>
   </si>
   <si>
-    <t>"^http://sws.geonames.org/(.*)"</t>
-  </si>
-  <si>
     <t>Le P87_is_identified_by sur les Places…</t>
   </si>
   <si>
@@ -749,6 +746,9 @@
   </si>
   <si>
     <t>( [ sh:class crmarch:A2_Stratigraphic_Volume_Unit ] [ sh:class crm:E22_Man-Made_Object ] )</t>
+  </si>
+  <si>
+    <t>"^https://sws.geonames.org/[0-9](.*)/$"</t>
   </si>
 </sst>
 </file>
@@ -1695,23 +1695,23 @@
     </row>
     <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
@@ -1735,7 +1735,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G23" t="s">
         <v>37</v>
@@ -1767,23 +1767,23 @@
     </row>
     <row r="25" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G25" t="s">
         <v>37</v>
@@ -1791,23 +1791,23 @@
     </row>
     <row r="26" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G26" t="s">
         <v>37</v>
@@ -1830,11 +1830,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ88"/>
+  <dimension ref="A1:AMJ87"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1987,119 +1987,141 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:1024" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11"/>
-      <c r="F11"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:1024" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="11" spans="1:1024" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L11" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M11" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="AMI12"/>
-      <c r="AMJ12"/>
-    </row>
-    <row r="13" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="O11" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="AMI11"/>
+      <c r="AMJ11"/>
+    </row>
+    <row r="12" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B12" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E12" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M12" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="N12" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="O12" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:1024" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>CONCATENATE("oash:P",ROW(A14))</f>
+        <v>oash:P14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B14, " sur un ", C14)</f>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14"/>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:1024" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>CONCATENATE("oash:P",ROW(A15))</f>
         <v>oash:P15</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -2109,24 +2131,26 @@
       </c>
       <c r="E15" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B15, " sur un ", C15)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Site</v>
+        <v>Contraintes de crm:P1_is_identified_by sur un oash:Site</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15"/>
+        <v>199</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:1024" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>CONCATENATE("oash:P",ROW(A16))</f>
         <v>oash:P16</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -2136,28 +2160,30 @@
       </c>
       <c r="E16" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B16, " sur un ", C16)</f>
-        <v>Contraintes de crm:P1_is_identified_by sur un oash:Site</v>
+        <v>Contraintes de skos:prefLabel sur un oash:Site</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>200</v>
+        <v>111</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:1024" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>112</v>
+      </c>
+      <c r="O16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>CONCATENATE("oash:P",ROW(A17))</f>
         <v>oash:P17</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
@@ -2165,74 +2191,74 @@
       </c>
       <c r="E17" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B17, " sur un ", C17)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:Site</v>
+        <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
+        <v>114</v>
+      </c>
+      <c r="G17"/>
+      <c r="I17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1024" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="str">
         <f>CONCATENATE("oash:P",ROW(A18))</f>
         <v>oash:P18</v>
       </c>
-      <c r="B18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B18, " sur un ", C18)</f>
-        <v>Contraintes de crm:P53_has_former_or_current_location sur un oash:Site</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18"/>
-      <c r="I18" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="N18" s="14" t="s">
+      <c r="C18" s="20"/>
+      <c r="F18" s="20" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:1024" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="str">
-        <f>CONCATENATE("oash:P",ROW(A19))</f>
-        <v>oash:P19</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="F19" s="20" t="s">
+      <c r="G18" s="20"/>
+      <c r="AMJ18"/>
+    </row>
+    <row r="19" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="AMJ19"/>
-    </row>
-    <row r="20" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+    </row>
+    <row r="20" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f>CONCATENATE("oash:P",ROW(A20))</f>
+        <v>oash:P20</v>
+      </c>
+      <c r="B20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B20, " sur un ", C20)</f>
+        <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>CONCATENATE("oash:P",ROW(A21))</f>
         <v>oash:P21</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>46</v>
@@ -2242,28 +2268,23 @@
       </c>
       <c r="E21" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B21, " sur un ", C21)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:EncounterEvent</v>
+        <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="N21" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="G21"/>
+      <c r="I21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>CONCATENATE("oash:P",ROW(A22))</f>
         <v>oash:P22</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>46</v>
@@ -2273,78 +2294,79 @@
       </c>
       <c r="E22" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B22, " sur un ", C22)</f>
-        <v>Contraintes de crm:P14_carried_out_by sur un oash:EncounterEvent</v>
+        <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="G22"/>
-      <c r="I22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="J22" s="13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>CONCATENATE("oash:P",ROW(A23))</f>
         <v>oash:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>220</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B23, " sur un ", C23)</f>
-        <v>Contraintes de crmsci:O19_has_found_object sur un oash:EncounterEvent</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="G23"/>
-      <c r="J23" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1024" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>CONCATENATE("oash:P",ROW(A24))</f>
-        <v>oash:P24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G24"/>
-      <c r="H24">
+      <c r="H23">
         <v>1</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I23" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>CONCATENATE("oash:P",ROW(A25))</f>
+        <v>oash:P25</v>
+      </c>
+      <c r="B25" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B25, " sur un ", C25)</f>
+        <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25"/>
+      <c r="I25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>CONCATENATE("oash:P",ROW(A26))</f>
         <v>oash:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>50</v>
@@ -2354,81 +2376,81 @@
       </c>
       <c r="E26" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B26, " sur un ", C26)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:Person</v>
+        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G26"/>
-      <c r="I26" t="s">
-        <v>43</v>
-      </c>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
+      <c r="I26" s="21"/>
+      <c r="J26" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1024" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="str">
         <f>CONCATENATE("oash:P",ROW(A27))</f>
         <v>oash:P27</v>
       </c>
-      <c r="B27" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="1" t="str">
+      <c r="D27" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="20" t="str">
         <f>CONCATENATE("Contraintes de ", B27, " sur un ", C27)</f>
-        <v>Contraintes de crm:P14i_performed sur un oash:Person</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G27"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="13" t="s">
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:1024" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="str">
+      <c r="G27" s="20"/>
+      <c r="I27" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="22"/>
+      <c r="AMJ27" s="18"/>
+    </row>
+    <row r="28" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
         <f>CONCATENATE("oash:P",ROW(A28))</f>
         <v>oash:P28</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="20" t="s">
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="20" t="str">
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B28, " sur un ", C28)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:Person</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="I28" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="22"/>
-      <c r="AMJ28" s="18"/>
-    </row>
-    <row r="29" spans="1:1024" ht="127.5" x14ac:dyDescent="0.2">
+        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28"/>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>CONCATENATE("oash:P",ROW(A29))</f>
         <v>oash:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
         <v>50</v>
       </c>
       <c r="D29" t="s">
@@ -2436,219 +2458,218 @@
       </c>
       <c r="E29" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B29, " sur un ", C29)</f>
-        <v>Contraintes de crm:P107i_is_current_or_former_member_of sur un oash:Person</v>
+        <v>Contraintes de skos:prefLabel sur un oash:Person</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G29"/>
-      <c r="I29" t="s">
-        <v>55</v>
-      </c>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:1024" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A30" t="str">
-        <f>CONCATENATE("oash:P",ROW(A30))</f>
-        <v>oash:P30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B30, " sur un ", C30)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:Person</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>112</v>
+      </c>
+      <c r="O29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>112</v>
-      </c>
-      <c r="O30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1024" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+    </row>
+    <row r="31" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>CONCATENATE("oash:P",ROW(A31))</f>
+        <v>oash:P31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B31, " sur un ", C31)</f>
+        <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:1024" ht="102" x14ac:dyDescent="0.2">
+      <c r="G31"/>
+      <c r="I31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1024" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>CONCATENATE("oash:P",ROW(A32))</f>
         <v>oash:P32</v>
       </c>
-      <c r="B32" t="s">
-        <v>126</v>
+      <c r="B32" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="C32" t="s">
         <v>54</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B32, " sur un ", C32)</f>
-        <v>Contraintes de crm:P131_is_identified_by sur un oash:LegalBody</v>
-      </c>
-      <c r="F32" s="1" t="s">
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>136</v>
       </c>
       <c r="G32"/>
-      <c r="I32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="I32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>CONCATENATE("oash:P",ROW(A33))</f>
         <v>oash:P33</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>106</v>
+      <c r="B33" t="s">
+        <v>110</v>
       </c>
       <c r="C33" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" t="s">
         <v>107</v>
       </c>
       <c r="E33" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B33, " sur un ", C33)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:LegalBody</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="G33"/>
-      <c r="I33" s="18" t="s">
+        <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f t="shared" ref="A35:A40" si="0">CONCATENATE("oash:P",ROW(A35))</f>
+        <v>oash:P35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" ref="E35:E40" si="1">CONCATENATE("Contraintes de ", B35, " sur un ", C35)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35"/>
+      <c r="K35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>oash:P36</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I36" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f>CONCATENATE("oash:P",ROW(A34))</f>
-        <v>oash:P34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B34, " sur un ", C34)</f>
-        <v>Contraintes de skos:prefLabel sur un oash:LegalBody</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
-        <v>112</v>
-      </c>
-      <c r="O34" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f t="shared" ref="A36:A41" si="0">CONCATENATE("oash:P",ROW(A36))</f>
-        <v>oash:P36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>141</v>
-      </c>
-      <c r="C36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="1" t="str">
-        <f t="shared" ref="E36:E41" si="1">CONCATENATE("Contraintes de ", B36, " sur un ", C36)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:BuiltWork</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G36"/>
-      <c r="K36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="str">
+      <c r="N36" s="19"/>
+    </row>
+    <row r="37" spans="1:15" s="21" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="str">
         <f t="shared" si="0"/>
         <v>oash:P37</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="18" t="s">
+      <c r="B37" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="20" t="str">
+      <c r="D37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:BuiltWork</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N37" s="19"/>
-    </row>
-    <row r="38" spans="1:15" s="21" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="str">
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>oash:P38</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" t="s">
         <v>107</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:BuiltWork</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>47</v>
+        <v>146</v>
+      </c>
+      <c r="G38"/>
+      <c r="N38" s="14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -2657,7 +2678,7 @@
         <v>oash:P39</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
         <v>58</v>
@@ -2667,23 +2688,23 @@
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:BuiltWork</v>
+        <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G39"/>
-      <c r="N39" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="I39" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>oash:P40</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>148</v>
+      <c r="B40" t="s">
+        <v>110</v>
       </c>
       <c r="C40" t="s">
         <v>58</v>
@@ -2693,114 +2714,114 @@
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:BuiltWork</v>
+        <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G40"/>
-      <c r="I40" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f t="shared" si="0"/>
-        <v>oash:P41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Contraintes de skos:prefLabel sur un oash:BuiltWork</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>112</v>
+      </c>
+      <c r="O40" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="K41" t="s">
+    </row>
+    <row r="42" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f t="shared" ref="A42:A49" si="2">CONCATENATE("oash:P",ROW(A42))</f>
+        <v>oash:P42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f t="shared" ref="E42:E49" si="3">CONCATENATE("Contraintes de ", B42, " sur un ", C42)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42"/>
+      <c r="K42" t="s">
         <v>112</v>
       </c>
-      <c r="O41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" ref="A43:A50" si="2">CONCATENATE("oash:P",ROW(A43))</f>
+        <f t="shared" si="2"/>
         <v>oash:P43</v>
       </c>
-      <c r="B43" t="s">
-        <v>141</v>
+      <c r="B43" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="C43" t="s">
         <v>62</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f t="shared" ref="E43:E50" si="3">CONCATENATE("Contraintes de ", B43, " sur un ", C43)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeFeature</v>
+        <f t="shared" si="3"/>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G43"/>
+      <c r="I43" t="s">
+        <v>39</v>
+      </c>
       <c r="K43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="2"/>
         <v>oash:P44</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" t="s">
         <v>107</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>153</v>
       </c>
       <c r="G44"/>
-      <c r="I44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="N44" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="2"/>
         <v>oash:P45</v>
       </c>
-      <c r="B45" s="21" t="s">
-        <v>146</v>
+      <c r="B45" t="s">
+        <v>118</v>
       </c>
       <c r="C45" t="s">
         <v>62</v>
@@ -2810,54 +2831,53 @@
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G45"/>
-      <c r="N45" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" s="21" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="str">
         <f t="shared" si="2"/>
         <v>oash:P46</v>
       </c>
-      <c r="B46" t="s">
-        <v>119</v>
+      <c r="B46" s="21" t="s">
+        <v>143</v>
       </c>
       <c r="C46" t="s">
         <v>62</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P2_has_type sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="M46" s="13" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" s="21" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="I46" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="str">
         <f t="shared" si="2"/>
         <v>oash:P47</v>
       </c>
-      <c r="B47" s="21" t="s">
-        <v>144</v>
+      <c r="B47" t="s">
+        <v>157</v>
       </c>
       <c r="C47" t="s">
         <v>62</v>
@@ -2867,48 +2887,50 @@
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>157</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="G47"/>
       <c r="I47" s="21" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="str">
+      <c r="A48" t="str">
         <f t="shared" si="2"/>
         <v>oash:P48</v>
       </c>
-      <c r="B48" t="s">
-        <v>158</v>
+      <c r="B48" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="C48" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" t="s">
         <v>107</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:ManMadeFeature</v>
+        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>159</v>
+        <v>235</v>
       </c>
       <c r="G48"/>
-      <c r="I48" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="I48" s="21"/>
+      <c r="J48" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" si="2"/>
         <v>oash:P49</v>
       </c>
-      <c r="B49" s="21" t="s">
-        <v>148</v>
+      <c r="B49" t="s">
+        <v>110</v>
       </c>
       <c r="C49" t="s">
         <v>62</v>
@@ -2918,60 +2940,59 @@
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>Contraintes de crm:P46_is_composed_of sur un oash:ManMadeFeature</v>
+        <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G49"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f t="shared" si="2"/>
-        <v>oash:P50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Contraintes de skos:prefLabel sur un oash:ManMadeFeature</v>
-      </c>
-      <c r="F50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
+        <v>112</v>
+      </c>
+      <c r="O49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="K50" t="s">
+    </row>
+    <row r="51" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A51" t="str">
+        <f t="shared" ref="A51:A59" si="4">CONCATENATE("oash:P",ROW(A51))</f>
+        <v>oash:P51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f t="shared" ref="E51:E59" si="5">CONCATENATE("Contraintes de ", B51, " sur un ", C51)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51"/>
+      <c r="K51" t="s">
         <v>112</v>
       </c>
-      <c r="O50" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f t="shared" ref="A52:A60" si="4">CONCATENATE("oash:P",ROW(A52))</f>
+        <f t="shared" si="4"/>
         <v>oash:P52</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
         <v>66</v>
@@ -2980,15 +3001,15 @@
         <v>107</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f t="shared" ref="E52:E60" si="5">CONCATENATE("Contraintes de ", B52, " sur un ", C52)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:ManMadeObject</v>
+        <f t="shared" si="5"/>
+        <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>163</v>
       </c>
       <c r="G52"/>
-      <c r="K52" t="s">
-        <v>112</v>
+      <c r="I52" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
@@ -2996,8 +3017,8 @@
         <f t="shared" si="4"/>
         <v>oash:P53</v>
       </c>
-      <c r="B53" t="s">
-        <v>109</v>
+      <c r="B53" s="21" t="s">
+        <v>145</v>
       </c>
       <c r="C53" t="s">
         <v>66</v>
@@ -3007,23 +3028,23 @@
       </c>
       <c r="E53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P1_is_identified_by sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>164</v>
       </c>
       <c r="G53"/>
-      <c r="I53" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="N53" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f t="shared" si="4"/>
         <v>oash:P54</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>146</v>
+      <c r="B54" t="s">
+        <v>165</v>
       </c>
       <c r="C54" t="s">
         <v>66</v>
@@ -3033,40 +3054,40 @@
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G54"/>
       <c r="N54" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="4"/>
         <v>oash:P55</v>
       </c>
-      <c r="B55" t="s">
-        <v>166</v>
+      <c r="B55" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="C55" t="s">
         <v>66</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P45_consists_of sur un oash:ManMadeObject</v>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>167</v>
       </c>
       <c r="G55"/>
-      <c r="N55" s="14" t="s">
-        <v>121</v>
+      <c r="I55" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -3075,7 +3096,7 @@
         <v>oash:P56</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
         <v>66</v>
@@ -3085,14 +3106,14 @@
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:ManMadeObject</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G56"/>
-      <c r="I56" t="s">
-        <v>39</v>
+      <c r="I56" s="21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
@@ -3101,7 +3122,7 @@
         <v>oash:P57</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
         <v>66</v>
@@ -3111,152 +3132,150 @@
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:ManMadeObject</v>
+        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="G57"/>
       <c r="I57" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="J57" s="13"/>
+    </row>
+    <row r="58" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f t="shared" si="4"/>
         <v>oash:P58</v>
       </c>
-      <c r="B58" s="21" t="s">
-        <v>170</v>
+      <c r="B58" t="s">
+        <v>157</v>
       </c>
       <c r="C58" t="s">
         <v>66</v>
       </c>
-      <c r="D58" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E58" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>Contraintes de crmarch:AP21i_is_contained_in sur un oash:ManMadeObject</v>
-      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G58"/>
-      <c r="I58" s="21" t="s">
-        <v>224</v>
+      <c r="I58" t="s">
+        <v>63</v>
       </c>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="4"/>
         <v>oash:P59</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
         <v>66</v>
       </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G59"/>
-      <c r="I59" t="s">
-        <v>63</v>
-      </c>
-      <c r="J59" s="13"/>
-    </row>
-    <row r="60" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A60" t="str">
-        <f t="shared" si="4"/>
-        <v>oash:P60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" t="s">
-        <v>66</v>
-      </c>
-      <c r="D60" t="s">
-        <v>107</v>
-      </c>
-      <c r="E60" s="1" t="str">
+      <c r="D59" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="1" t="str">
         <f t="shared" si="5"/>
         <v>Contraintes de skos:prefLabel sur un oash:ManMadeObject</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>112</v>
+      </c>
+      <c r="O59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f t="shared" ref="A61:A67" si="6">CONCATENATE("oash:P",ROW(A61))</f>
+        <v>oash:P61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" t="s">
+        <v>222</v>
+      </c>
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f t="shared" ref="E61:E67" si="7">CONCATENATE("Contraintes de ", B61, " sur un ", C61)</f>
+        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="K60" t="s">
+      <c r="G61"/>
+      <c r="K61" t="s">
         <v>112</v>
       </c>
-      <c r="O60" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f t="shared" ref="A62:A68" si="6">CONCATENATE("oash:P",ROW(A62))</f>
+        <f t="shared" si="6"/>
         <v>oash:P62</v>
       </c>
-      <c r="B62" t="s">
-        <v>141</v>
+      <c r="B62" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>223</v>
-      </c>
-      <c r="D62" t="s">
+        <v>222</v>
+      </c>
+      <c r="D62" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f t="shared" ref="E62:E68" si="7">CONCATENATE("Contraintes de ", B62, " sur un ", C62)</f>
-        <v>Contraintes de crm:P3_has_note sur un oash:StratigraphicVolumeUnit</v>
+        <f t="shared" si="7"/>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G62"/>
-      <c r="K62" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f t="shared" si="6"/>
         <v>oash:P63</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="C63" t="s">
-        <v>223</v>
-      </c>
-      <c r="D63" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="D63" t="s">
         <v>107</v>
       </c>
       <c r="E63" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F63" s="1" t="s">
+        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F63" s="20" t="s">
         <v>173</v>
       </c>
       <c r="G63"/>
-      <c r="I63" t="s">
-        <v>39</v>
-      </c>
+      <c r="M63" s="18"/>
     </row>
     <row r="64" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
@@ -3264,156 +3283,163 @@
         <v>oash:P64</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D64" t="s">
         <v>107</v>
       </c>
       <c r="E64" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P101_had_as_general_use sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F64" s="20" t="s">
+        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicVolumeUnit</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G64"/>
-      <c r="M64" s="18"/>
-    </row>
-    <row r="65" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f t="shared" si="6"/>
         <v>oash:P65</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C65" t="s">
-        <v>223</v>
-      </c>
-      <c r="D65" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E65" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmarch:AP21_contains sur un oash:StratigraphicVolumeUnit</v>
+        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
+      <c r="G65"/>
       <c r="I65" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f t="shared" si="6"/>
         <v>oash:P66</v>
       </c>
-      <c r="B66" s="21" t="s">
-        <v>144</v>
+      <c r="B66" t="s">
+        <v>157</v>
       </c>
       <c r="C66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>107</v>
       </c>
       <c r="E66" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crmsci:O19i_was_object_found_by sur un oash:StratigraphicVolumeUnit</v>
+        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>176</v>
       </c>
       <c r="G66"/>
-      <c r="I66" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f t="shared" si="6"/>
         <v>oash:P67</v>
       </c>
       <c r="B67" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>223</v>
-      </c>
-      <c r="D67" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="D67" t="s">
         <v>107</v>
       </c>
       <c r="E67" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>Contraintes de crm:P46i_forms_part_of sur un oash:StratigraphicVolumeUnit</v>
+        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G67"/>
-      <c r="I67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" t="str">
-        <f t="shared" si="6"/>
-        <v>oash:P68</v>
-      </c>
-      <c r="B68" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" t="s">
-        <v>223</v>
-      </c>
-      <c r="D68" t="s">
-        <v>107</v>
-      </c>
-      <c r="E68" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>Contraintes de skos:prefLabel sur un oash:StratigraphicVolumeUnit</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="O67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="G68">
+    </row>
+    <row r="69" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" t="str">
+        <f t="shared" ref="A69:A74" si="8">CONCATENATE("oash:P",ROW(A69))</f>
+        <v>oash:P69</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D69" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B69, " sur un ", C69)</f>
+        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G69" s="1">
         <v>1</v>
       </c>
-      <c r="O68" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="J69" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
-        <f t="shared" ref="A70:A75" si="8">CONCATENATE("oash:P",ROW(A70))</f>
+        <f t="shared" si="8"/>
         <v>oash:P70</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D70" t="s">
         <v>107</v>
       </c>
       <c r="E70" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B70, " sur un ", C70)</f>
-        <v>Contraintes de [ sh:alternativePath (crm:P8_took_place_on_or_within [ sh:inversePath crm:P8i_witnessed ]) ] sur un oash:EncounterEvent, oash:Event</v>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -3421,41 +3447,43 @@
       <c r="H70">
         <v>1</v>
       </c>
-      <c r="J70" s="13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>71</v>
+      </c>
+      <c r="J70" s="13"/>
+    </row>
+    <row r="71" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f t="shared" si="8"/>
         <v>oash:P71</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>181</v>
+        <v>70</v>
       </c>
       <c r="D71" t="s">
         <v>107</v>
       </c>
       <c r="E71" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B71, " sur un ", C71)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:EncounterEvent, oash:Event</v>
+        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G71" s="1">
-        <v>1</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="G71"/>
       <c r="H71">
         <v>1</v>
       </c>
-      <c r="I71" t="s">
-        <v>71</v>
-      </c>
       <c r="J71" s="13"/>
+      <c r="K71" t="s">
+        <v>112</v>
+      </c>
+      <c r="L71" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="72" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
@@ -3463,7 +3491,7 @@
         <v>oash:P72</v>
       </c>
       <c r="B72" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>70</v>
@@ -3473,10 +3501,10 @@
       </c>
       <c r="E72" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B72, " sur un ", C72)</f>
-        <v>Contraintes de crm:P82a_begin_of_the_begin sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G72"/>
       <c r="H72">
@@ -3487,16 +3515,16 @@
         <v>112</v>
       </c>
       <c r="L72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="114.75" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
         <f t="shared" si="8"/>
         <v>oash:P73</v>
       </c>
       <c r="B73" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>70</v>
@@ -3506,176 +3534,169 @@
       </c>
       <c r="E73" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B73, " sur un ", C73)</f>
-        <v>Contraintes de crm:P82b_end_of_the_end sur un oash:TimeSpanEvent</v>
+        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G73"/>
+        <v>189</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
       <c r="H73">
         <v>1</v>
       </c>
-      <c r="J73" s="13"/>
-      <c r="K73" t="s">
-        <v>112</v>
-      </c>
-      <c r="L73" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="89.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f t="shared" si="8"/>
         <v>oash:P74</v>
       </c>
-      <c r="B74" t="s">
-        <v>189</v>
+      <c r="B74" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D74" t="s">
-        <v>107</v>
-      </c>
-      <c r="E74" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B74, " sur un ", C74)</f>
-        <v>Contraintes de rdfs:label sur un oash:TimeSpanEvent</v>
-      </c>
       <c r="F74" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G74">
+        <v>198</v>
+      </c>
+      <c r="G74" s="1">
         <v>1</v>
       </c>
-      <c r="H74">
+    </row>
+    <row r="75" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f>CONCATENATE("oash:P",ROW(A76))</f>
+        <v>oash:P76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A75" t="str">
-        <f t="shared" si="8"/>
-        <v>oash:P75</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G75" s="1">
+      <c r="E76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" s="23" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>CONCATENATE("oash:P",ROW(A77))</f>
         <v>oash:P77</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D77" t="s">
+        <v>107</v>
+      </c>
+      <c r="E77" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B77, " sur un ", C77)</f>
+        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D77" s="1">
-        <v>1</v>
-      </c>
-      <c r="E77" t="s">
-        <v>43</v>
-      </c>
-      <c r="F77" s="1" t="s">
+      <c r="G77"/>
+      <c r="I77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" t="str">
+        <f t="shared" ref="A78:A83" si="9">CONCATENATE("oash:P",ROW(A78))</f>
+        <v>oash:P78</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G77" s="1">
-        <v>1</v>
-      </c>
-      <c r="I77" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" t="str">
-        <f>CONCATENATE("oash:P",ROW(A78))</f>
-        <v>oash:P78</v>
-      </c>
-      <c r="B78" t="s">
-        <v>106</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D78" t="s">
         <v>107</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
-        <v>Contraintes de crm:P48_has_preferred_identifier sur un oash:E31_Document</v>
+        <f t="shared" ref="E78" si="10">CONCATENATE("Contraintes de ", B78, " sur un ", C78)</f>
+        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>208</v>
       </c>
       <c r="G78"/>
-      <c r="I78" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="N78" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
-        <f t="shared" ref="A79:A84" si="9">CONCATENATE("oash:P",ROW(A79))</f>
+        <f t="shared" si="9"/>
         <v>oash:P79</v>
       </c>
-      <c r="B79" s="21" t="s">
-        <v>119</v>
+      <c r="B79" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D79" t="s">
-        <v>107</v>
-      </c>
-      <c r="E79" s="1" t="str">
-        <f t="shared" ref="E79" si="10">CONCATENATE("Contraintes de ", B79, " sur un ", C79)</f>
-        <v>Contraintes de crm:P2_has_type sur un oash:E31_Document</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G79"/>
-      <c r="H79">
+        <v>232</v>
+      </c>
+      <c r="G79">
         <v>1</v>
       </c>
-      <c r="N79" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J79" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="N79" s="14"/>
+    </row>
+    <row r="80" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
         <f t="shared" si="9"/>
         <v>oash:P80</v>
       </c>
       <c r="B80" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" t="s">
         <v>210</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="G80">
         <v>1</v>
       </c>
-      <c r="J80" s="13" t="s">
-        <v>234</v>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="N80" s="14"/>
     </row>
@@ -3685,128 +3706,130 @@
         <v>oash:P81</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G81"/>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N81" s="14"/>
     </row>
-    <row r="82" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
         <f t="shared" si="9"/>
         <v>oash:P82</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>219</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G82"/>
-      <c r="H82">
-        <v>1</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>202</v>
-      </c>
+      <c r="I82" t="s">
+        <v>51</v>
+      </c>
+      <c r="J82" s="13"/>
       <c r="N82" s="14"/>
     </row>
-    <row r="83" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f t="shared" si="9"/>
         <v>oash:P83</v>
       </c>
-      <c r="B83" s="13" t="s">
-        <v>122</v>
+      <c r="B83" t="s">
+        <v>181</v>
       </c>
       <c r="C83" t="s">
-        <v>211</v>
-      </c>
-      <c r="E83" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="D83" t="s">
+        <v>107</v>
+      </c>
+      <c r="E83" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B83, " sur un ", C83)</f>
+        <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
+      </c>
       <c r="F83" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G83"/>
+      <c r="H83">
+        <v>1</v>
+      </c>
       <c r="I83" t="s">
-        <v>51</v>
-      </c>
-      <c r="J83" s="13"/>
+        <v>71</v>
+      </c>
       <c r="N83" s="14"/>
     </row>
-    <row r="84" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" t="str">
-        <f t="shared" si="9"/>
-        <v>oash:P84</v>
-      </c>
-      <c r="B84" t="s">
-        <v>182</v>
-      </c>
-      <c r="C84" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" t="s">
-        <v>107</v>
-      </c>
-      <c r="E84" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B84, " sur un ", C84)</f>
-        <v>Contraintes de crm:P4_has_time-span sur un oash:DocumentCreation</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H84">
+    <row r="84" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C84"/>
+      <c r="E84" s="1"/>
+      <c r="N84" s="14"/>
+    </row>
+    <row r="85" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A86" t="str">
+        <f>CONCATENATE("oash:P",ROW(A86))</f>
+        <v>oash:P86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>188</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D86" t="s">
+        <v>107</v>
+      </c>
+      <c r="E86" s="1" t="str">
+        <f>CONCATENATE("Contraintes de ", B86, " sur un ", C86)</f>
+        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G86" s="1">
         <v>1</v>
       </c>
-      <c r="I84" t="s">
-        <v>71</v>
-      </c>
-      <c r="N84" s="14"/>
-    </row>
-    <row r="85" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85"/>
-      <c r="E85" s="1"/>
-      <c r="N85" s="14"/>
-    </row>
-    <row r="86" spans="1:14" s="23" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="K86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>CONCATENATE("oash:P",ROW(A87))</f>
         <v>oash:P87</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D87" t="s">
         <v>107</v>
       </c>
       <c r="E87" s="1" t="str">
         <f>CONCATENATE("Contraintes de ", B87, " sur un ", C87)</f>
-        <v>Contraintes de rdfs:label sur un oash:PreferredIdentifier</v>
+        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>192</v>
@@ -3815,34 +3838,6 @@
         <v>1</v>
       </c>
       <c r="K87" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A88" t="str">
-        <f>CONCATENATE("oash:P",ROW(A88))</f>
-        <v>oash:P88</v>
-      </c>
-      <c r="B88" t="s">
-        <v>189</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D88" t="s">
-        <v>107</v>
-      </c>
-      <c r="E88" s="1" t="str">
-        <f>CONCATENATE("Contraintes de ", B88, " sur un ", C88)</f>
-        <v>Contraintes de rdfs:label sur un oash:Appellation</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G88" s="1">
-        <v>1</v>
-      </c>
-      <c r="K88" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3850,14 +3845,14 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="C8" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="N18" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="N21" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="N39" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="N45" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="N54" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="N55" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="N79" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="N17" r:id="rId4" display="&quot;^http://sws.geonames.org/(.*)&quot;" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="N20" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="N38" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N44" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="N53" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="N54" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="N78" r:id="rId10" xr:uid="{04CAA37E-B745-4E5A-878B-48652F622BBE}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>